<commit_message>
Embibe :: Updated gobal search test data, segmentio test data and signuppage.java
</commit_message>
<xml_diff>
--- a/Embibe/test-data/SegmentIoData.xlsx
+++ b/Embibe/test-data/SegmentIoData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="570" windowWidth="14055" windowHeight="4050" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="510" yWindow="570" windowWidth="14055" windowHeight="4050" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,11 @@
     <sheet name="system-events" sheetId="7" r:id="rId7"/>
     <sheet name="footer" sheetId="8" r:id="rId8"/>
     <sheet name="header" sheetId="9" r:id="rId9"/>
-    <sheet name="Main" sheetId="10" r:id="rId10"/>
+    <sheet name="headerResults" sheetId="10" r:id="rId10"/>
+    <sheet name="Results" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">header!$B$1:$AC$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">header!$A$1:$AB$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'learn-page'!$D$1:$D$1000</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'search-home-page'!$D$1:$D$1000</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'search-result-page'!$D$1:$D$1038</definedName>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="703">
   <si>
     <t>event_code</t>
   </si>
@@ -2703,26 +2704,71 @@
     <t>r-header-41</t>
   </si>
   <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Event Code</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Unique Value</t>
+    <t>e_event_code</t>
+  </si>
+  <si>
+    <t>e_log_type</t>
+  </si>
+  <si>
+    <t>e_event_name</t>
+  </si>
+  <si>
+    <t>e_nav_element</t>
+  </si>
+  <si>
+    <t>e_event_type</t>
+  </si>
+  <si>
+    <t>e_intent_to_pay</t>
+  </si>
+  <si>
+    <t>e_extra_params</t>
+  </si>
+  <si>
+    <t>a_log_type</t>
+  </si>
+  <si>
+    <t>log_type_result</t>
+  </si>
+  <si>
+    <t>a_event_name</t>
+  </si>
+  <si>
+    <t>event_name_result</t>
+  </si>
+  <si>
+    <t>a_nav_element</t>
+  </si>
+  <si>
+    <t>nav_element_result</t>
+  </si>
+  <si>
+    <t>a_event_type</t>
+  </si>
+  <si>
+    <t>event_type_result</t>
+  </si>
+  <si>
+    <t>a_intent_to_pay</t>
+  </si>
+  <si>
+    <t>intent_to_pay_result</t>
+  </si>
+  <si>
+    <t>a_extra_params</t>
+  </si>
+  <si>
+    <t>extra_params_result</t>
+  </si>
+  <si>
+    <t>- email- mobile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2804,6 +2850,12 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2837,7 +2889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2971,7 +3023,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6502,347 +6561,1788 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="69" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.42578125" style="69" customWidth="1"/>
+    <col min="8" max="8" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15" style="69" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.140625" style="69" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.42578125" style="69" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:19">
       <c r="A1" s="67" t="s">
-        <v>683</v>
+        <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
+        <v>684</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>690</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>691</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>693</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>686</v>
+      </c>
+      <c r="I1" s="68" t="s">
+        <v>694</v>
+      </c>
+      <c r="J1" s="68" t="s">
+        <v>695</v>
+      </c>
+      <c r="K1" s="67" t="s">
         <v>687</v>
       </c>
-      <c r="C1" s="67" t="s">
-        <v>684</v>
-      </c>
-      <c r="D1" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="67" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B2" s="66" t="s">
+      <c r="L1" s="68" t="s">
+        <v>696</v>
+      </c>
+      <c r="M1" s="68" t="s">
+        <v>697</v>
+      </c>
+      <c r="N1" s="67" t="s">
+        <v>688</v>
+      </c>
+      <c r="O1" s="68" t="s">
+        <v>698</v>
+      </c>
+      <c r="P1" s="68" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q1" s="67" t="s">
+        <v>689</v>
+      </c>
+      <c r="R1" s="68" t="s">
+        <v>700</v>
+      </c>
+      <c r="S1" s="68" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="70" t="s">
         <v>614</v>
       </c>
-      <c r="C2" s="66" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B3" s="66" t="s">
+      <c r="B2" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="70"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="70" t="s">
         <v>615</v>
       </c>
-      <c r="C3" s="66" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B4" s="66" t="s">
+      <c r="B3" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="70"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="70" t="s">
         <v>616</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B5" s="66" t="s">
+      <c r="B4" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E4" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="70"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="70" t="s">
         <v>617</v>
       </c>
-      <c r="C5" s="66" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B6" s="66" t="s">
+      <c r="B5" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="70"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="70" t="s">
         <v>618</v>
       </c>
-      <c r="C6" s="66" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B7" s="66" t="s">
+      <c r="B6" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E6" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="70"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="70" t="s">
         <v>620</v>
       </c>
-      <c r="C7" s="66" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B8" s="66" t="s">
+      <c r="B7" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="70"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="70" t="s">
         <v>621</v>
       </c>
-      <c r="C8" s="66" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B9" s="66" t="s">
+      <c r="B8" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="70"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="70" t="s">
         <v>622</v>
       </c>
-      <c r="C9" s="66" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B10" s="66" t="s">
+      <c r="B9" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E9" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="70"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="70" t="s">
         <v>623</v>
       </c>
-      <c r="C10" s="66" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B11" s="66" t="s">
+      <c r="B10" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E10" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="70"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="70" t="s">
         <v>635</v>
       </c>
-      <c r="C11" s="66" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B12" s="66" t="s">
+      <c r="B11" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>224</v>
+      </c>
+      <c r="H11" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="70"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="70" t="s">
         <v>639</v>
       </c>
-      <c r="C12" s="66" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B13" s="66" t="s">
+      <c r="B12" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>239</v>
+      </c>
+      <c r="H12" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="70" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="70" t="s">
         <v>640</v>
       </c>
-      <c r="C13" s="66" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B14" s="66" t="s">
+      <c r="B13" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E13" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="70"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="70" t="s">
         <v>652</v>
       </c>
-      <c r="C14" s="66" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B15" s="66" t="s">
+      <c r="B14" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="K14" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="70" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="70" t="s">
         <v>653</v>
       </c>
-      <c r="C15" s="66" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B16" s="66" t="s">
+      <c r="B15" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E15" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="70" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="70" t="s">
         <v>654</v>
       </c>
-      <c r="C16" s="66" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B17" s="66" t="s">
+      <c r="B16" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="H16" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="K16" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="70"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="70" t="s">
         <v>655</v>
       </c>
-      <c r="C17" s="66" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B18" s="66" t="s">
+      <c r="B17" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="H17" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="K17" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="70" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="70" t="s">
         <v>662</v>
       </c>
-      <c r="C18" s="66" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B19" s="66" t="s">
+      <c r="B18" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="K18" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="70"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="70" t="s">
         <v>663</v>
       </c>
-      <c r="C19" s="66" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B20" s="66" t="s">
+      <c r="B19" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E19" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="K19" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="70" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="70" t="s">
         <v>666</v>
       </c>
-      <c r="C20" s="66" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B21" s="66" t="s">
+      <c r="B20" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E20" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="H20" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="K20" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="70" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="70" t="s">
         <v>667</v>
       </c>
-      <c r="C21" s="66" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B22" s="66" t="s">
+      <c r="B21" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="K21" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="70"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="70" t="s">
         <v>673</v>
       </c>
-      <c r="C22" s="66" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B23" s="66" t="s">
+      <c r="B22" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E22" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="K22" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N22" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="70"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="70" t="s">
         <v>674</v>
       </c>
-      <c r="C23" s="66" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B24" s="66" t="s">
+      <c r="B23" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E23" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="H23" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="K23" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="70"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="70" t="s">
         <v>675</v>
       </c>
-      <c r="C24" s="66" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B25" s="66" t="s">
+      <c r="B24" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E24" s="70" t="s">
+        <v>193</v>
+      </c>
+      <c r="H24" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="K24" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="70"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="70" t="s">
         <v>676</v>
       </c>
-      <c r="C25" s="66" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B26" s="7" t="s">
+      <c r="B25" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>259</v>
+      </c>
+      <c r="H25" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="K25" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="70" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="72" t="s">
         <v>678</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B27" s="66" t="s">
+      <c r="B26" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="H26" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="70" t="s">
         <v>679</v>
       </c>
-      <c r="C27" s="66" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B28" s="66" t="s">
+      <c r="B27" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E27" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="H27" s="72" t="s">
+        <v>680</v>
+      </c>
+      <c r="K27" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="70" t="s">
         <v>681</v>
       </c>
-      <c r="C28" s="66" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="67" t="s">
-        <v>685</v>
-      </c>
-      <c r="B29" s="66" t="s">
+      <c r="B28" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E28" s="72" t="s">
+        <v>541</v>
+      </c>
+      <c r="H28" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="70" t="s">
         <v>682</v>
       </c>
-      <c r="C29" s="66" t="s">
-        <v>682</v>
+      <c r="B29" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="H29" s="72" t="s">
+        <v>553</v>
+      </c>
+      <c r="K29" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" s="72">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A2" s="66" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="66">
+        <v>0</v>
+      </c>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A3" s="66" t="s">
+        <v>615</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="66">
+        <v>0</v>
+      </c>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
+      <c r="X3" s="66"/>
+      <c r="Y3" s="66"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A4" s="66" t="s">
+        <v>616</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="66">
+        <v>0</v>
+      </c>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A5" s="66" t="s">
+        <v>617</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="66">
+        <v>0</v>
+      </c>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
+      <c r="Y5" s="66"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A6" s="66" t="s">
+        <v>618</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="66">
+        <v>0</v>
+      </c>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="66"/>
+      <c r="T6" s="66"/>
+      <c r="U6" s="66"/>
+      <c r="V6" s="66"/>
+      <c r="W6" s="66"/>
+      <c r="X6" s="66"/>
+      <c r="Y6" s="66"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A7" s="66" t="s">
+        <v>620</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="66">
+        <v>0</v>
+      </c>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="66"/>
+      <c r="V7" s="66"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="66"/>
+      <c r="Y7" s="66"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="66" t="s">
+        <v>621</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="66">
+        <v>0</v>
+      </c>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="66"/>
+      <c r="T8" s="66"/>
+      <c r="U8" s="66"/>
+      <c r="V8" s="66"/>
+      <c r="W8" s="66"/>
+      <c r="X8" s="66"/>
+      <c r="Y8" s="66"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A9" s="66" t="s">
+        <v>622</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="66">
+        <v>0</v>
+      </c>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A10" s="66" t="s">
+        <v>623</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="66">
+        <v>0</v>
+      </c>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
+      <c r="U10" s="66"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A11" s="66" t="s">
+        <v>635</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="66">
+        <v>0</v>
+      </c>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="66" t="s">
+        <v>639</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="66">
+        <v>0</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>240</v>
+      </c>
+      <c r="H12" s="66"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
+      <c r="S12" s="66"/>
+      <c r="T12" s="66"/>
+      <c r="U12" s="66"/>
+      <c r="V12" s="66"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="66"/>
+      <c r="Y12" s="66"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="66" t="s">
+        <v>640</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="65">
+        <v>0</v>
+      </c>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="66"/>
+      <c r="V13" s="66"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="66"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A14" s="66" t="s">
+        <v>652</v>
+      </c>
+      <c r="B14" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="65">
+        <v>0</v>
+      </c>
+      <c r="G14" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
+      <c r="U14" s="66"/>
+      <c r="V14" s="66"/>
+      <c r="W14" s="66"/>
+      <c r="X14" s="66"/>
+      <c r="Y14" s="66"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="66" t="s">
+        <v>653</v>
+      </c>
+      <c r="B15" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="65">
+        <v>0</v>
+      </c>
+      <c r="G15" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" s="66"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="66"/>
+      <c r="W15" s="66"/>
+      <c r="X15" s="66"/>
+      <c r="Y15" s="66"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="66" t="s">
+        <v>654</v>
+      </c>
+      <c r="B16" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="65">
+        <v>0</v>
+      </c>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="66"/>
+      <c r="X16" s="66"/>
+      <c r="Y16" s="66"/>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A17" s="66" t="s">
+        <v>655</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="65">
+        <v>0</v>
+      </c>
+      <c r="G17" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" s="66"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
+      <c r="U17" s="66"/>
+      <c r="V17" s="66"/>
+      <c r="W17" s="66"/>
+      <c r="X17" s="66"/>
+      <c r="Y17" s="66"/>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A18" s="66" t="s">
+        <v>662</v>
+      </c>
+      <c r="B18" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="65">
+        <v>0</v>
+      </c>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
+      <c r="U18" s="66"/>
+      <c r="V18" s="66"/>
+      <c r="W18" s="66"/>
+      <c r="X18" s="66"/>
+      <c r="Y18" s="66"/>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A19" s="66" t="s">
+        <v>663</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="65">
+        <v>0</v>
+      </c>
+      <c r="G19" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="66"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
+      <c r="U19" s="66"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="66"/>
+      <c r="X19" s="66"/>
+      <c r="Y19" s="66"/>
+    </row>
+    <row r="20" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A20" s="66" t="s">
+        <v>666</v>
+      </c>
+      <c r="B20" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="65">
+        <v>0</v>
+      </c>
+      <c r="G20" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" s="66"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="66"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="66"/>
+      <c r="R20" s="66"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="66"/>
+      <c r="U20" s="66"/>
+      <c r="V20" s="66"/>
+      <c r="W20" s="66"/>
+      <c r="X20" s="66"/>
+      <c r="Y20" s="66"/>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A21" s="66" t="s">
+        <v>667</v>
+      </c>
+      <c r="B21" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C21" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="E21" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="65">
+        <v>0</v>
+      </c>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="66"/>
+      <c r="U21" s="66"/>
+      <c r="V21" s="66"/>
+      <c r="W21" s="66"/>
+      <c r="X21" s="66"/>
+      <c r="Y21" s="66"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A22" s="66" t="s">
+        <v>673</v>
+      </c>
+      <c r="B22" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="65">
+        <v>0</v>
+      </c>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="66"/>
+      <c r="Y22" s="66"/>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A23" s="66" t="s">
+        <v>674</v>
+      </c>
+      <c r="B23" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C23" s="66" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="65">
+        <v>0</v>
+      </c>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="66"/>
+      <c r="Y23" s="66"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A24" s="66" t="s">
+        <v>675</v>
+      </c>
+      <c r="B24" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="65">
+        <v>0</v>
+      </c>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
+      <c r="U24" s="66"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="66"/>
+      <c r="X24" s="66"/>
+      <c r="Y24" s="66"/>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A25" s="66" t="s">
+        <v>676</v>
+      </c>
+      <c r="B25" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>259</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="65">
+        <v>0</v>
+      </c>
+      <c r="G25" s="66" t="s">
+        <v>260</v>
+      </c>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="66"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
+      <c r="S25" s="66"/>
+      <c r="T25" s="66"/>
+      <c r="U25" s="66"/>
+      <c r="V25" s="66"/>
+      <c r="W25" s="66"/>
+      <c r="X25" s="66"/>
+      <c r="Y25" s="66"/>
+    </row>
+    <row r="26" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="B26" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A27" s="66" t="s">
+        <v>679</v>
+      </c>
+      <c r="B27" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A28" s="66" t="s">
+        <v>681</v>
+      </c>
+      <c r="B28" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="D28" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A29" s="66" t="s">
+        <v>682</v>
+      </c>
+      <c r="B29" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -48897,59 +50397,57 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC50"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="44" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>688</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>689</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="6"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -48965,37 +50463,34 @@
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-    </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A2" s="66" t="s">
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>614</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>609</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="8">
+      <c r="F2" s="8">
         <v>0</v>
       </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="12"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -49011,37 +50506,34 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A3" s="66" t="s">
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>615</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>609</v>
+        <v>49</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="8">
+      <c r="F3" s="8">
         <v>0</v>
       </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="6"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -49057,37 +50549,34 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A4" s="66" t="s">
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>616</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>609</v>
+        <v>56</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="8">
         <v>0</v>
       </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="6"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -49103,37 +50592,34 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A5" s="66" t="s">
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>617</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>609</v>
+        <v>64</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="8">
+      <c r="F5" s="8">
         <v>0</v>
       </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="6"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -49149,37 +50635,34 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A6" s="66" t="s">
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>618</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>609</v>
+        <v>70</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="8">
+      <c r="F6" s="8">
         <v>0</v>
       </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="6"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -49195,35 +50678,32 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:29" ht="15.75" hidden="1" customHeight="1">
-      <c r="A7" s="66" t="s">
+    </row>
+    <row r="7" spans="1:28" ht="15.75" hidden="1" customHeight="1">
+      <c r="A7" s="8" t="s">
         <v>619</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>609</v>
+        <v>74</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="8">
+      <c r="F7" s="8">
         <v>0</v>
       </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="6"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -49239,37 +50719,34 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A8" s="66" t="s">
+    </row>
+    <row r="8" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>620</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>609</v>
+        <v>49</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="8">
+      <c r="F8" s="8">
         <v>0</v>
       </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="6"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -49285,37 +50762,34 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A9" s="66" t="s">
+    </row>
+    <row r="9" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>621</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>621</v>
+        <v>609</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>609</v>
+        <v>56</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="8">
+      <c r="F9" s="8">
         <v>0</v>
       </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="6"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -49331,37 +50805,34 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A10" s="66" t="s">
+    </row>
+    <row r="10" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>622</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>609</v>
+        <v>64</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="8">
+      <c r="F10" s="8">
         <v>0</v>
       </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="6"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -49377,37 +50848,34 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A11" s="66" t="s">
+    </row>
+    <row r="11" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>623</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>609</v>
+        <v>70</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="8">
+      <c r="F11" s="8">
         <v>0</v>
       </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="6"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -49423,35 +50891,32 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:29" ht="15.75" hidden="1" customHeight="1">
-      <c r="A12" s="66" t="s">
+    </row>
+    <row r="12" spans="1:28" ht="15.75" hidden="1" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>628</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>628</v>
+        <v>609</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>609</v>
+        <v>74</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="8">
+      <c r="F12" s="8">
         <v>0</v>
       </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
@@ -49467,33 +50932,30 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-    </row>
-    <row r="13" spans="1:29" ht="15.75" hidden="1" customHeight="1">
-      <c r="A13" s="66" t="s">
+    </row>
+    <row r="13" spans="1:28" ht="15.75" hidden="1" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>630</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>630</v>
+        <v>609</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>609</v>
+        <v>96</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="8">
+      <c r="F13" s="8">
         <v>0</v>
       </c>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -49511,33 +50973,30 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-    </row>
-    <row r="14" spans="1:29" ht="15.75" hidden="1" customHeight="1">
-      <c r="A14" s="66" t="s">
+    </row>
+    <row r="14" spans="1:28" ht="15.75" hidden="1" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>633</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>633</v>
+        <v>609</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>609</v>
+        <v>222</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>222</v>
+        <v>40</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="8">
+      <c r="F14" s="8">
         <v>0</v>
       </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -49555,35 +51014,32 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-    </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A15" s="66" t="s">
+    </row>
+    <row r="15" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>635</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>635</v>
+        <v>609</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>609</v>
+        <v>224</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>224</v>
+        <v>40</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="8">
+      <c r="F15" s="8">
         <v>0</v>
       </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="8" t="s">
+      <c r="I15" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -49601,35 +51057,32 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-    </row>
-    <row r="16" spans="1:29" ht="15.75" hidden="1" customHeight="1">
-      <c r="A16" s="66" t="s">
+    </row>
+    <row r="16" spans="1:28" ht="15.75" hidden="1" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>637</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>637</v>
+        <v>609</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>609</v>
+        <v>236</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>236</v>
+        <v>40</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="8">
+      <c r="F16" s="8">
         <v>0</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="8"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -49647,39 +51100,36 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-    </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A17" s="66" t="s">
+    </row>
+    <row r="17" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>639</v>
+        <v>609</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>609</v>
+        <v>239</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="8">
+      <c r="F17" s="8">
         <v>0</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8" t="s">
+      <c r="H17" s="8"/>
+      <c r="I17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="54"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -49695,37 +51145,34 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-    </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A18" s="66" t="s">
+    </row>
+    <row r="18" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>640</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="C18" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="65">
+      <c r="F18" s="65">
         <v>0</v>
       </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="6"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -49740,35 +51187,32 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-    </row>
-    <row r="19" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A19" s="66" t="s">
+    </row>
+    <row r="19" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>650</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>650</v>
-      </c>
-      <c r="C19" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C19" s="56" t="s">
+        <v>253</v>
+      </c>
       <c r="D19" s="56" t="s">
-        <v>253</v>
+        <v>40</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="65">
+      <c r="F19" s="65">
         <v>0</v>
       </c>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="6"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -49783,37 +51227,34 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-    </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A20" s="66" t="s">
+    </row>
+    <row r="20" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>652</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>652</v>
-      </c>
-      <c r="C20" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C20" s="56" t="s">
+        <v>142</v>
+      </c>
       <c r="D20" s="56" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E20" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="65">
+      <c r="F20" s="65">
         <v>0</v>
       </c>
-      <c r="H20" s="56" t="s">
+      <c r="G20" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="8" t="s">
+      <c r="H20" s="3"/>
+      <c r="I20" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -49831,39 +51272,36 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-    </row>
-    <row r="21" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A21" s="66" t="s">
+    </row>
+    <row r="21" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A21" s="8" t="s">
         <v>653</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>653</v>
-      </c>
-      <c r="C21" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="D21" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="62">
+      <c r="F21" s="62">
         <v>0</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="8" t="s">
+      <c r="H21" s="3"/>
+      <c r="I21" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="18"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -49879,37 +51317,34 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-    </row>
-    <row r="22" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A22" s="66" t="s">
+    </row>
+    <row r="22" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A22" s="8" t="s">
         <v>654</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>654</v>
-      </c>
-      <c r="C22" s="8" t="s">
         <v>609</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="62">
+      <c r="F22" s="62">
         <v>0</v>
       </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="18"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -49925,39 +51360,36 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-    </row>
-    <row r="23" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A23" s="66" t="s">
+    </row>
+    <row r="23" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A23" s="8" t="s">
         <v>655</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>655</v>
-      </c>
-      <c r="C23" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C23" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="62">
+      <c r="F23" s="62">
         <v>0</v>
       </c>
-      <c r="H23" s="66" t="s">
+      <c r="G23" s="66" t="s">
         <v>174</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="8" t="s">
+      <c r="H23" s="3"/>
+      <c r="I23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="54"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -49973,37 +51405,34 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-    </row>
-    <row r="24" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A24" s="66" t="s">
+    </row>
+    <row r="24" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A24" s="8" t="s">
         <v>662</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>662</v>
-      </c>
-      <c r="C24" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C24" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="D24" s="3" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="62">
+      <c r="F24" s="62">
         <v>0</v>
       </c>
+      <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="18"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -50019,39 +51448,36 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
-    </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A25" s="66" t="s">
+    </row>
+    <row r="25" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A25" s="8" t="s">
         <v>663</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>663</v>
-      </c>
-      <c r="C25" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C25" s="56" t="s">
+        <v>142</v>
+      </c>
       <c r="D25" s="56" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="E25" s="56" t="s">
-        <v>184</v>
-      </c>
-      <c r="F25" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="65">
+      <c r="F25" s="65">
         <v>0</v>
       </c>
-      <c r="H25" s="56" t="s">
+      <c r="G25" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="8" t="s">
+      <c r="H25" s="3"/>
+      <c r="I25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="18"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -50067,30 +51493,27 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
-      <c r="AB25" s="3"/>
-    </row>
-    <row r="26" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A26" s="66" t="s">
+    </row>
+    <row r="26" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A26" s="8" t="s">
         <v>665</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>665</v>
-      </c>
-      <c r="C26" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="62">
+      <c r="F26" s="62">
         <v>0</v>
       </c>
+      <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -50111,39 +51534,36 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-    </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A27" s="66" t="s">
+    </row>
+    <row r="27" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A27" s="8" t="s">
         <v>666</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>666</v>
-      </c>
-      <c r="C27" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C27" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="D27" s="3" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="62">
+      <c r="F27" s="62">
         <v>0</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="8" t="s">
+      <c r="H27" s="3"/>
+      <c r="I27" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="54"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -50159,35 +51579,32 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
-      <c r="AB27" s="3"/>
-    </row>
-    <row r="28" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A28" s="66" t="s">
+    </row>
+    <row r="28" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>667</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="C28" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E28" s="66" t="s">
+      <c r="D28" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="62">
+      <c r="F28" s="62">
         <v>0</v>
       </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="8" t="s">
+      <c r="I28" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -50205,36 +51622,33 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
-      <c r="AB28" s="3"/>
-    </row>
-    <row r="29" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A29" s="66" t="s">
+    </row>
+    <row r="29" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A29" s="8" t="s">
         <v>668</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>668</v>
-      </c>
-      <c r="C29" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="D29" s="3" t="s">
-        <v>193</v>
+        <v>226</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G29" s="62">
+      <c r="F29" s="62">
         <v>0</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>195</v>
       </c>
+      <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="66"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
@@ -50251,33 +51665,30 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
-    </row>
-    <row r="30" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A30" s="66" t="s">
+    </row>
+    <row r="30" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A30" s="8" t="s">
         <v>669</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>669</v>
-      </c>
-      <c r="C30" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C30" s="3" t="s">
+        <v>229</v>
+      </c>
       <c r="D30" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="62">
+      <c r="F30" s="62">
         <v>0</v>
       </c>
-      <c r="H30" s="66" t="s">
+      <c r="G30" s="66" t="s">
         <v>230</v>
       </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -50297,33 +51708,30 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
-      <c r="AB30" s="3"/>
-    </row>
-    <row r="31" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A31" s="66" t="s">
+    </row>
+    <row r="31" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A31" s="8" t="s">
         <v>670</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>670</v>
-      </c>
-      <c r="C31" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C31" s="3" t="s">
+        <v>232</v>
+      </c>
       <c r="D31" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="62">
+      <c r="F31" s="62">
         <v>0</v>
       </c>
+      <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -50341,33 +51749,30 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
-      <c r="AB31" s="3"/>
-    </row>
-    <row r="32" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A32" s="66" t="s">
+    </row>
+    <row r="32" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A32" s="8" t="s">
         <v>671</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>671</v>
-      </c>
-      <c r="C32" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C32" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="D32" s="3" t="s">
-        <v>144</v>
+        <v>233</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="62">
+      <c r="F32" s="62">
         <v>0</v>
       </c>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -50385,30 +51790,27 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
-      <c r="AB32" s="3"/>
-    </row>
-    <row r="33" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A33" s="66" t="s">
+    </row>
+    <row r="33" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A33" s="8" t="s">
         <v>672</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>672</v>
-      </c>
-      <c r="C33" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C33" s="3" t="s">
+        <v>244</v>
+      </c>
       <c r="D33" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="62">
+      <c r="F33" s="62">
         <v>0</v>
       </c>
+      <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -50429,37 +51831,34 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
-      <c r="AB33" s="3"/>
-    </row>
-    <row r="34" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A34" s="66" t="s">
+    </row>
+    <row r="34" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A34" s="8" t="s">
         <v>673</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>673</v>
-      </c>
-      <c r="C34" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C34" s="3" t="s">
+        <v>247</v>
+      </c>
       <c r="D34" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="62">
+      <c r="F34" s="62">
         <v>0</v>
       </c>
+      <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="54"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
@@ -50475,37 +51874,34 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
-    </row>
-    <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="66" t="s">
+    </row>
+    <row r="35" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A35" s="8" t="s">
         <v>674</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>674</v>
-      </c>
-      <c r="C35" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="D35" s="56" t="s">
+      <c r="C35" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="E35" s="66" t="s">
+      <c r="D35" s="66" t="s">
         <v>144</v>
       </c>
-      <c r="F35" s="56" t="s">
+      <c r="E35" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="65">
+      <c r="F35" s="65">
         <v>0</v>
       </c>
-      <c r="H35" s="56"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="8" t="s">
+      <c r="G35" s="56"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="18"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
@@ -50521,35 +51917,32 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
-      <c r="AB35" s="3"/>
-    </row>
-    <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="66" t="s">
+    </row>
+    <row r="36" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A36" s="8" t="s">
         <v>675</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>675</v>
-      </c>
-      <c r="C36" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C36" s="56" t="s">
+        <v>193</v>
+      </c>
       <c r="D36" s="56" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E36" s="56" t="s">
-        <v>184</v>
-      </c>
-      <c r="F36" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G36" s="65">
+      <c r="F36" s="65">
         <v>0</v>
       </c>
+      <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="8" t="s">
+      <c r="I36" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -50567,37 +51960,34 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
-      <c r="AB36" s="3"/>
-    </row>
-    <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="66" t="s">
+    </row>
+    <row r="37" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A37" s="8" t="s">
         <v>676</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>676</v>
-      </c>
-      <c r="C37" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C37" s="56" t="s">
+        <v>259</v>
+      </c>
       <c r="D37" s="56" t="s">
-        <v>259</v>
+        <v>184</v>
       </c>
       <c r="E37" s="56" t="s">
-        <v>184</v>
-      </c>
-      <c r="F37" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="65">
+      <c r="F37" s="65">
         <v>0</v>
       </c>
-      <c r="H37" s="66" t="s">
+      <c r="G37" s="66" t="s">
         <v>260</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="8" t="s">
+      <c r="H37" s="3"/>
+      <c r="I37" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -50615,35 +52005,32 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
       <c r="AA37" s="3"/>
-      <c r="AB37" s="3"/>
-    </row>
-    <row r="38" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A38" s="66" t="s">
+    </row>
+    <row r="38" spans="1:27" ht="15.75" hidden="1" customHeight="1">
+      <c r="A38" s="8" t="s">
         <v>677</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>677</v>
-      </c>
-      <c r="C38" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C38" s="56" t="s">
+        <v>202</v>
+      </c>
       <c r="D38" s="56" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="E38" s="56" t="s">
-        <v>184</v>
-      </c>
-      <c r="F38" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="65">
+      <c r="F38" s="65">
         <v>0</v>
       </c>
+      <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="54"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
@@ -50659,124 +52046,111 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
-      <c r="AB38" s="3"/>
-    </row>
-    <row r="39" spans="1:28" ht="15.75" customHeight="1">
+    </row>
+    <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>678</v>
-      </c>
-      <c r="C39" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>609</v>
       </c>
+      <c r="C39" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="D39" s="7" t="s">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A40" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A41" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="E41" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="7">
+      <c r="F41" s="7">
         <v>0</v>
       </c>
-      <c r="J39" s="7" t="s">
+      <c r="I41" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="66" t="s">
-        <v>679</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="C40" s="8" t="s">
+    <row r="42" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A42" s="8" t="s">
+        <v>682</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>680</v>
-      </c>
-      <c r="F40" s="7" t="s">
+      <c r="D42" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G40" s="7">
+      <c r="F42" s="7">
         <v>0</v>
       </c>
-      <c r="J40" s="7" t="s">
+      <c r="I42" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A41" s="66" t="s">
-        <v>681</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>681</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>609</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41" s="7">
-        <v>0</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A42" s="66" t="s">
-        <v>682</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>682</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>609</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>553</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G42" s="7">
-        <v>0</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="44" spans="1:28" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="45" spans="1:28" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="46" spans="1:28" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="47" spans="1:28" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="48" spans="1:28" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="49" spans="9:9" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="50" spans="9:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="I50" s="7"/>
+    <row r="43" spans="1:27" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="44" spans="1:27" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="45" spans="1:27" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="46" spans="1:27" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="47" spans="1:27" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="48" spans="1:27" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="49" spans="8:8" ht="15.75" hidden="1" customHeight="1"/>
+    <row r="50" spans="8:8" ht="15.75" hidden="1" customHeight="1">
+      <c r="H50" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AC50">
+  <autoFilter ref="A1:AB50">
     <filterColumn colId="8">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>

</xml_diff>